<commit_message>
Changing the Industry records with — sign to empty cell and exporting again the excel file which is clean
</commit_message>
<xml_diff>
--- a/cleaned_data_df_2018.xlsx
+++ b/cleaned_data_df_2018.xlsx
@@ -2211,11 +2211,7 @@
           <t>MissMalini Entertainment</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -3621,11 +3617,7 @@
           <t>Jagaran Microfin</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr">
         <is>
           <t>Debt Financing</t>
@@ -4101,11 +4093,7 @@
           <t>FLEECA</t>
         </is>
       </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B123" t="inlineStr"/>
       <c r="C123" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -4851,11 +4839,7 @@
           <t>WheelsEMI</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B148" t="inlineStr"/>
       <c r="C148" t="inlineStr">
         <is>
           <t>Series B</t>
@@ -5061,11 +5045,7 @@
           <t>Fric Bergen</t>
         </is>
       </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B155" t="inlineStr"/>
       <c r="C155" t="inlineStr">
         <is>
           <t>Venture - Series Unknown</t>
@@ -5691,11 +5671,7 @@
           <t>Deftouch</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B176" t="inlineStr"/>
       <c r="C176" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -5901,11 +5877,7 @@
           <t>Corefactors</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B183" t="inlineStr"/>
       <c r="C183" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -6771,11 +6743,7 @@
           <t>Cell Propulsion</t>
         </is>
       </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B212" t="inlineStr"/>
       <c r="C212" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -7371,11 +7339,7 @@
           <t>Flathalt</t>
         </is>
       </c>
-      <c r="B232" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B232" t="inlineStr"/>
       <c r="C232" t="inlineStr">
         <is>
           <t>Angel</t>
@@ -7521,11 +7485,7 @@
           <t>dishq</t>
         </is>
       </c>
-      <c r="B237" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B237" t="inlineStr"/>
       <c r="C237" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -7611,11 +7571,7 @@
           <t>Trell</t>
         </is>
       </c>
-      <c r="B240" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B240" t="inlineStr"/>
       <c r="C240" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -7731,11 +7687,7 @@
           <t>HousingMan.com</t>
         </is>
       </c>
-      <c r="B244" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B244" t="inlineStr"/>
       <c r="C244" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -7761,11 +7713,7 @@
           <t>Steradian Semiconductors</t>
         </is>
       </c>
-      <c r="B245" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B245" t="inlineStr"/>
       <c r="C245" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -7881,11 +7829,7 @@
           <t>SaffronStays</t>
         </is>
       </c>
-      <c r="B249" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B249" t="inlineStr"/>
       <c r="C249" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -8001,11 +7945,7 @@
           <t>Inner Being Wellness</t>
         </is>
       </c>
-      <c r="B253" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B253" t="inlineStr"/>
       <c r="C253" t="inlineStr">
         <is>
           <t>Angel</t>
@@ -8181,11 +8121,7 @@
           <t>MySEODoc</t>
         </is>
       </c>
-      <c r="B259" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B259" t="inlineStr"/>
       <c r="C259" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -8211,11 +8147,7 @@
           <t>ENLYFT DIGITAL SOLUTIONS PRIVATE LIMITED</t>
         </is>
       </c>
-      <c r="B260" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B260" t="inlineStr"/>
       <c r="C260" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -8241,11 +8173,7 @@
           <t>Scale Labs</t>
         </is>
       </c>
-      <c r="B261" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B261" t="inlineStr"/>
       <c r="C261" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -9291,11 +9219,7 @@
           <t>Roadcast</t>
         </is>
       </c>
-      <c r="B296" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B296" t="inlineStr"/>
       <c r="C296" t="inlineStr">
         <is>
           <t>Angel</t>
@@ -10221,11 +10145,7 @@
           <t>Toffee</t>
         </is>
       </c>
-      <c r="B327" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B327" t="inlineStr"/>
       <c r="C327" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -10251,11 +10171,7 @@
           <t>ORO Wealth</t>
         </is>
       </c>
-      <c r="B328" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B328" t="inlineStr"/>
       <c r="C328" t="inlineStr">
         <is>
           <t>Series A</t>
@@ -10851,11 +10767,7 @@
           <t>Finwego</t>
         </is>
       </c>
-      <c r="B348" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B348" t="inlineStr"/>
       <c r="C348" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -12381,11 +12293,7 @@
           <t>Cred</t>
         </is>
       </c>
-      <c r="B399" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B399" t="inlineStr"/>
       <c r="C399" t="inlineStr">
         <is>
           <t>Seed</t>
@@ -14151,11 +14059,7 @@
           <t>Origo</t>
         </is>
       </c>
-      <c r="B458" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B458" t="inlineStr"/>
       <c r="C458" t="inlineStr">
         <is>
           <t>Venture - Series Unknown</t>
@@ -14601,11 +14505,7 @@
           <t>Sequretek</t>
         </is>
       </c>
-      <c r="B473" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B473" t="inlineStr"/>
       <c r="C473" t="inlineStr">
         <is>
           <t>Venture - Series Unknown</t>
@@ -14631,11 +14531,7 @@
           <t>Avenues Payments India Pvt. Ltd.</t>
         </is>
       </c>
-      <c r="B474" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B474" t="inlineStr"/>
       <c r="C474" t="inlineStr">
         <is>
           <t>Corporate Round</t>
@@ -14721,11 +14617,7 @@
           <t>Planet11 eCommerce Solutions India (Avenue11)</t>
         </is>
       </c>
-      <c r="B477" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B477" t="inlineStr"/>
       <c r="C477" t="inlineStr">
         <is>
           <t>Corporate Round</t>
@@ -14781,11 +14673,7 @@
           <t>Iba Halal Care</t>
         </is>
       </c>
-      <c r="B479" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B479" t="inlineStr"/>
       <c r="C479" t="inlineStr">
         <is>
           <t>Series A</t>
@@ -14841,11 +14729,7 @@
           <t>Togedr</t>
         </is>
       </c>
-      <c r="B481" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B481" t="inlineStr"/>
       <c r="C481" t="inlineStr">
         <is>
           <t>Venture - Series Unknown</t>
@@ -15741,11 +15625,7 @@
           <t>Scholify</t>
         </is>
       </c>
-      <c r="B511" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
+      <c r="B511" t="inlineStr"/>
       <c r="C511" t="inlineStr">
         <is>
           <t>Pre-Seed</t>

</xml_diff>